<commit_message>
Scraping the company name, Customer ID, Invoice Number, and the date
</commit_message>
<xml_diff>
--- a/ScrapedInvoiceData.xlsx
+++ b/ScrapedInvoiceData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\UiPath\PdfDataScraping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69952EA8-BD68-4AD8-A2E8-EFFDAC640185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +356,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write the scraping data into excel sheet
</commit_message>
<xml_diff>
--- a/ScrapedInvoiceData.xlsx
+++ b/ScrapedInvoiceData.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\UiPath\PdfDataScraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69952EA8-BD68-4AD8-A2E8-EFFDAC640185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694550F4-A026-4D47-8402-6E28DBA49A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,13 +30,13 @@
     <t>Company Name</t>
   </si>
   <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
     <t>Invoice Number</t>
   </si>
   <si>
     <t>Total Amount</t>
-  </si>
-  <si>
-    <t>Customer ID</t>
   </si>
   <si>
     <t>Date</t>
@@ -46,13 +46,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,8 +81,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,36 +370,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>